<commit_message>
Update Monitoreo Nuevos Productos.xlsx
</commit_message>
<xml_diff>
--- a/Monitoreo Nuevos Productos.xlsx
+++ b/Monitoreo Nuevos Productos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karen\Dropbox\DI Monitoreo II\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298AEDBB-C25F-47C8-9E56-268DDDAA09F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478A9A03-5FD8-4263-97EC-263FF6074DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{3C601918-C683-4A9E-9764-2E2F3DE6B565}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{3C601918-C683-4A9E-9764-2E2F3DE6B565}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitoreo Nuevos Productos" sheetId="1" r:id="rId1"/>
@@ -1313,111 +1313,7 @@
     <cellStyle name="Millares" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="618">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="608">
     <dxf>
       <font>
         <strike val="0"/>
@@ -7222,27 +7118,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8AB307C7-AF39-4578-A163-A8BC847F650D}" name="Tabla1" displayName="Tabla1" ref="A10:R96" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8AB307C7-AF39-4578-A163-A8BC847F650D}" name="Tabla1" displayName="Tabla1" ref="A10:R96" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A10:R96" xr:uid="{BE3B9459-9CC4-4B42-85DE-65D6DD89527B}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{AEA8EF0D-25C7-4111-8A9F-0B18B1765250}" name="SECTOR" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{752FAE73-6FD3-44CD-87CD-9043950F7C57}" name="COLECCIÓN" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{6007294C-E2A9-42FC-8D1B-04F4C15E7E6C}" name="TABLA MADRE" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{CC128664-1A0A-4FA0-9E24-7F2D50AC3945}" name="RESPONSABLE" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{47097AA3-BED4-48AF-B9DE-ABBBAEBF8480}" name="ESTADO" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{D1D0198B-6B8E-4844-BFB3-0C4C39A5DEEB}" name="TEMA" dataDxfId="22"/>
-    <tableColumn id="18" xr3:uid="{FCDE1CEA-9D32-4512-8B1E-E0F36B0D06E6}" name="En contenido" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{F7C33F71-D2AC-440D-B0A6-B78933C8E65D}" name="TIPO PRODUCTO" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{D2B9DAD1-8888-4EAE-B08D-DDAAD4D91214}" name="NOMBRE" dataDxfId="19"/>
-    <tableColumn id="9" xr3:uid="{B13359B5-127C-4ACD-BA41-0F932FFA47DE}" name="Cantidad" dataDxfId="18"/>
-    <tableColumn id="10" xr3:uid="{22126FF6-1849-455F-A6A6-7D65468619C8}" name="Títulos revisados" dataDxfId="17"/>
-    <tableColumn id="11" xr3:uid="{C4B2B2EE-05E3-4BD3-9138-0C5123EACD36}" name="Título Genérico - Shopify" dataDxfId="16"/>
-    <tableColumn id="12" xr3:uid="{48638419-EFAD-40F5-8E0C-171981824999}" name="Título específico" dataDxfId="15"/>
-    <tableColumn id="13" xr3:uid="{5E5D6E60-EE68-4304-B67C-4D8F2081F5C6}" name="Tags" dataDxfId="14"/>
-    <tableColumn id="14" xr3:uid="{4A7DE2E9-92D4-4649-893E-C2F9E0C999C9}" name="Link" dataDxfId="13" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="15" xr3:uid="{C604366C-A935-413E-B0A6-F9D41B311156}" name="Estado URL" dataDxfId="12"/>
-    <tableColumn id="16" xr3:uid="{E1C0300E-6E4D-4041-9E44-893F2242AEB3}" name="Responsable Revisión" dataDxfId="11"/>
-    <tableColumn id="17" xr3:uid="{B21BEC12-2A8B-4811-AA41-623D1FDA90AE}" name="Tags2" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{AEA8EF0D-25C7-4111-8A9F-0B18B1765250}" name="SECTOR" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{752FAE73-6FD3-44CD-87CD-9043950F7C57}" name="COLECCIÓN" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{6007294C-E2A9-42FC-8D1B-04F4C15E7E6C}" name="TABLA MADRE" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{CC128664-1A0A-4FA0-9E24-7F2D50AC3945}" name="RESPONSABLE" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{47097AA3-BED4-48AF-B9DE-ABBBAEBF8480}" name="ESTADO" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{D1D0198B-6B8E-4844-BFB3-0C4C39A5DEEB}" name="TEMA" dataDxfId="12"/>
+    <tableColumn id="18" xr3:uid="{FCDE1CEA-9D32-4512-8B1E-E0F36B0D06E6}" name="En contenido" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{F7C33F71-D2AC-440D-B0A6-B78933C8E65D}" name="TIPO PRODUCTO" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{D2B9DAD1-8888-4EAE-B08D-DDAAD4D91214}" name="NOMBRE" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{B13359B5-127C-4ACD-BA41-0F932FFA47DE}" name="Cantidad" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{22126FF6-1849-455F-A6A6-7D65468619C8}" name="Títulos revisados" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{C4B2B2EE-05E3-4BD3-9138-0C5123EACD36}" name="Título Genérico - Shopify" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{48638419-EFAD-40F5-8E0C-171981824999}" name="Título específico" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{5E5D6E60-EE68-4304-B67C-4D8F2081F5C6}" name="Tags" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{4A7DE2E9-92D4-4649-893E-C2F9E0C999C9}" name="Link" dataDxfId="3" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="15" xr3:uid="{C604366C-A935-413E-B0A6-F9D41B311156}" name="Estado URL" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{E1C0300E-6E4D-4041-9E44-893F2242AEB3}" name="Responsable Revisión" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{B21BEC12-2A8B-4811-AA41-623D1FDA90AE}" name="Tags2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7548,10 +7444,10 @@
   <dimension ref="A8:R111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="10" topLeftCell="D74" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="10" topLeftCell="K29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="A97" sqref="A97"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12476,1812 +12372,1812 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="L41:M44">
-    <cfRule type="expression" dxfId="617" priority="984">
+    <cfRule type="expression" dxfId="607" priority="984">
       <formula>#REF!="Reporte 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="616" priority="985">
+    <cfRule type="expression" dxfId="606" priority="985">
       <formula>#REF!="Reporte 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="615" priority="986">
+    <cfRule type="expression" dxfId="605" priority="986">
       <formula>#REF!="Informe 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="614" priority="987">
+    <cfRule type="expression" dxfId="604" priority="987">
       <formula>#REF!="Informe 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="613" priority="988">
+    <cfRule type="expression" dxfId="603" priority="988">
       <formula>#REF!="Informe 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="612" priority="989">
+    <cfRule type="expression" dxfId="602" priority="989">
       <formula>#REF!="Informe 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="611" priority="990">
+    <cfRule type="expression" dxfId="601" priority="990">
       <formula>#REF!="Informe 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="610" priority="991">
+    <cfRule type="expression" dxfId="600" priority="991">
       <formula>#REF!="Informe 5"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="609" priority="992">
+    <cfRule type="expression" dxfId="599" priority="992">
       <formula>#REF!="Informe 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="608" priority="993">
+    <cfRule type="expression" dxfId="598" priority="993">
       <formula>#REF!="Informe 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="607" priority="994">
+    <cfRule type="expression" dxfId="597" priority="994">
       <formula>#REF!="Informe 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="606" priority="995">
+    <cfRule type="expression" dxfId="596" priority="995">
       <formula>#REF!="Informe 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="605" priority="996">
+    <cfRule type="expression" dxfId="595" priority="996">
       <formula>#REF!="Gráfico 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="604" priority="997">
+    <cfRule type="expression" dxfId="594" priority="997">
       <formula>#REF!="Gráfico 25"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="603" priority="998">
+    <cfRule type="expression" dxfId="593" priority="998">
       <formula>#REF!="Gráfico 24"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="602" priority="999">
+    <cfRule type="expression" dxfId="592" priority="999">
       <formula>#REF!="Gráfico 23"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="601" priority="1000">
+    <cfRule type="expression" dxfId="591" priority="1000">
       <formula>#REF!="Gráfico 22"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="600" priority="1001">
+    <cfRule type="expression" dxfId="590" priority="1001">
       <formula>#REF!="Gráfico 21"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="599" priority="1002">
+    <cfRule type="expression" dxfId="589" priority="1002">
       <formula>#REF!="Gráfico 20"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="598" priority="1003">
+    <cfRule type="expression" dxfId="588" priority="1003">
       <formula>#REF!="Gráfico 18"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="597" priority="1004">
+    <cfRule type="expression" dxfId="587" priority="1004">
       <formula>#REF!="Gráfico 19"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="596" priority="1005">
+    <cfRule type="expression" dxfId="586" priority="1005">
       <formula>#REF!="Gráfico 17"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="595" priority="1006">
+    <cfRule type="expression" dxfId="585" priority="1006">
       <formula>#REF!="Gráfico 16"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="594" priority="1007">
+    <cfRule type="expression" dxfId="584" priority="1007">
       <formula>#REF!="Gráfico 15"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="593" priority="1008">
+    <cfRule type="expression" dxfId="583" priority="1008">
       <formula>#REF!="Gráfico 14"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="592" priority="1009">
+    <cfRule type="expression" dxfId="582" priority="1009">
       <formula>#REF!="Gráfico 12"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="591" priority="1010">
+    <cfRule type="expression" dxfId="581" priority="1010">
       <formula>#REF!="Gráfico 13"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="590" priority="1011">
+    <cfRule type="expression" dxfId="580" priority="1011">
       <formula>#REF!="Gráfico 11"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="589" priority="1012">
+    <cfRule type="expression" dxfId="579" priority="1012">
       <formula>#REF!="Gráfico 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="588" priority="1013">
+    <cfRule type="expression" dxfId="578" priority="1013">
       <formula>#REF!="Gráfico 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="587" priority="1014">
+    <cfRule type="expression" dxfId="577" priority="1014">
       <formula>#REF!="Gráfico 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="586" priority="1015">
+    <cfRule type="expression" dxfId="576" priority="1015">
       <formula>#REF!="Gráfico 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="585" priority="1016">
+    <cfRule type="expression" dxfId="575" priority="1016">
       <formula>#REF!="Gráfico 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="584" priority="1017">
+    <cfRule type="expression" dxfId="574" priority="1017">
       <formula>#REF!="Gráfico 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="583" priority="1018">
+    <cfRule type="expression" dxfId="573" priority="1018">
       <formula>#REF!="Gráfico 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="582" priority="1019">
+    <cfRule type="expression" dxfId="572" priority="1019">
       <formula>#REF!="Gráfico 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="581" priority="1020">
+    <cfRule type="expression" dxfId="571" priority="1020">
       <formula>#REF!="Gráfico 5"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J104:K2999">
-    <cfRule type="cellIs" dxfId="580" priority="982" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="570" priority="982" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N21:N32">
-    <cfRule type="expression" dxfId="579" priority="608">
+    <cfRule type="expression" dxfId="569" priority="608">
       <formula>$AD12="Reporte 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="578" priority="609">
+    <cfRule type="expression" dxfId="568" priority="609">
       <formula>$AD12="Reporte 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="577" priority="610">
+    <cfRule type="expression" dxfId="567" priority="610">
       <formula>$AD12="Informe 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="576" priority="611">
+    <cfRule type="expression" dxfId="566" priority="611">
       <formula>$AD12="Informe 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="575" priority="612">
+    <cfRule type="expression" dxfId="565" priority="612">
       <formula>$AD12="Informe 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="574" priority="613">
+    <cfRule type="expression" dxfId="564" priority="613">
       <formula>$AD12="Informe 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="573" priority="614">
+    <cfRule type="expression" dxfId="563" priority="614">
       <formula>$AD12="Informe 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="572" priority="615">
+    <cfRule type="expression" dxfId="562" priority="615">
       <formula>$AD12="Informe 5"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="571" priority="616">
+    <cfRule type="expression" dxfId="561" priority="616">
       <formula>$AD12="Informe 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="570" priority="617">
+    <cfRule type="expression" dxfId="560" priority="617">
       <formula>$AD12="Informe 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="569" priority="618">
+    <cfRule type="expression" dxfId="559" priority="618">
       <formula>$AD12="Informe 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="568" priority="619">
+    <cfRule type="expression" dxfId="558" priority="619">
       <formula>$AD12="Informe 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="567" priority="620">
+    <cfRule type="expression" dxfId="557" priority="620">
       <formula>$AD12="Gráfico 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="566" priority="621">
+    <cfRule type="expression" dxfId="556" priority="621">
       <formula>$AD12="Gráfico 25"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="565" priority="622">
+    <cfRule type="expression" dxfId="555" priority="622">
       <formula>$AD12="Gráfico 24"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="564" priority="623">
+    <cfRule type="expression" dxfId="554" priority="623">
       <formula>$AD12="Gráfico 23"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="563" priority="624">
+    <cfRule type="expression" dxfId="553" priority="624">
       <formula>$AD12="Gráfico 22"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="562" priority="625">
+    <cfRule type="expression" dxfId="552" priority="625">
       <formula>$AD12="Gráfico 21"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="561" priority="626">
+    <cfRule type="expression" dxfId="551" priority="626">
       <formula>$AD12="Gráfico 20"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="560" priority="627">
+    <cfRule type="expression" dxfId="550" priority="627">
       <formula>$AD12="Gráfico 18"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="559" priority="628">
+    <cfRule type="expression" dxfId="549" priority="628">
       <formula>$AD12="Gráfico 19"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="558" priority="629">
+    <cfRule type="expression" dxfId="548" priority="629">
       <formula>$AD12="Gráfico 17"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="557" priority="630">
+    <cfRule type="expression" dxfId="547" priority="630">
       <formula>$AD12="Gráfico 16"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="556" priority="631">
+    <cfRule type="expression" dxfId="546" priority="631">
       <formula>$AD12="Gráfico 15"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="555" priority="632">
+    <cfRule type="expression" dxfId="545" priority="632">
       <formula>$AD12="Gráfico 14"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="554" priority="633">
+    <cfRule type="expression" dxfId="544" priority="633">
       <formula>$AD12="Gráfico 12"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="553" priority="634">
+    <cfRule type="expression" dxfId="543" priority="634">
       <formula>$AD12="Gráfico 13"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="552" priority="635">
+    <cfRule type="expression" dxfId="542" priority="635">
       <formula>$AD12="Gráfico 11"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="551" priority="636">
+    <cfRule type="expression" dxfId="541" priority="636">
       <formula>$AD12="Gráfico 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="550" priority="637">
+    <cfRule type="expression" dxfId="540" priority="637">
       <formula>$AD12="Gráfico 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="549" priority="638">
+    <cfRule type="expression" dxfId="539" priority="638">
       <formula>$AD12="Gráfico 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="548" priority="639">
+    <cfRule type="expression" dxfId="538" priority="639">
       <formula>$AD12="Gráfico 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="547" priority="640">
+    <cfRule type="expression" dxfId="537" priority="640">
       <formula>$AD12="Gráfico 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="546" priority="641">
+    <cfRule type="expression" dxfId="536" priority="641">
       <formula>$AD12="Gráfico 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="545" priority="642">
+    <cfRule type="expression" dxfId="535" priority="642">
       <formula>$AD12="Gráfico 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="544" priority="643">
+    <cfRule type="expression" dxfId="534" priority="643">
       <formula>$AD12="Gráfico 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="543" priority="644">
+    <cfRule type="expression" dxfId="533" priority="644">
       <formula>$AD12="Gráfico 5"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N41:N48 N53:N56">
-    <cfRule type="expression" dxfId="542" priority="571">
+    <cfRule type="expression" dxfId="532" priority="571">
       <formula>$AD41="Reporte 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="541" priority="572">
+    <cfRule type="expression" dxfId="531" priority="572">
       <formula>$AD41="Reporte 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="540" priority="573">
+    <cfRule type="expression" dxfId="530" priority="573">
       <formula>$AD41="Informe 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="539" priority="574">
+    <cfRule type="expression" dxfId="529" priority="574">
       <formula>$AD41="Informe 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="538" priority="575">
+    <cfRule type="expression" dxfId="528" priority="575">
       <formula>$AD41="Informe 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="537" priority="576">
+    <cfRule type="expression" dxfId="527" priority="576">
       <formula>$AD41="Informe 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="536" priority="577">
+    <cfRule type="expression" dxfId="526" priority="577">
       <formula>$AD41="Informe 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="535" priority="578">
+    <cfRule type="expression" dxfId="525" priority="578">
       <formula>$AD41="Informe 5"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="534" priority="579">
+    <cfRule type="expression" dxfId="524" priority="579">
       <formula>$AD41="Informe 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="533" priority="580">
+    <cfRule type="expression" dxfId="523" priority="580">
       <formula>$AD41="Informe 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="532" priority="581">
+    <cfRule type="expression" dxfId="522" priority="581">
       <formula>$AD41="Informe 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="531" priority="582">
+    <cfRule type="expression" dxfId="521" priority="582">
       <formula>$AD41="Informe 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="530" priority="583">
+    <cfRule type="expression" dxfId="520" priority="583">
       <formula>$AD41="Gráfico 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="529" priority="584">
+    <cfRule type="expression" dxfId="519" priority="584">
       <formula>$AD41="Gráfico 25"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="528" priority="585">
+    <cfRule type="expression" dxfId="518" priority="585">
       <formula>$AD41="Gráfico 24"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="527" priority="586">
+    <cfRule type="expression" dxfId="517" priority="586">
       <formula>$AD41="Gráfico 23"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="526" priority="587">
+    <cfRule type="expression" dxfId="516" priority="587">
       <formula>$AD41="Gráfico 22"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="525" priority="588">
+    <cfRule type="expression" dxfId="515" priority="588">
       <formula>$AD41="Gráfico 21"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="524" priority="589">
+    <cfRule type="expression" dxfId="514" priority="589">
       <formula>$AD41="Gráfico 20"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="523" priority="590">
+    <cfRule type="expression" dxfId="513" priority="590">
       <formula>$AD41="Gráfico 18"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="522" priority="591">
+    <cfRule type="expression" dxfId="512" priority="591">
       <formula>$AD41="Gráfico 19"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="521" priority="592">
+    <cfRule type="expression" dxfId="511" priority="592">
       <formula>$AD41="Gráfico 17"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="520" priority="593">
+    <cfRule type="expression" dxfId="510" priority="593">
       <formula>$AD41="Gráfico 16"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="519" priority="594">
+    <cfRule type="expression" dxfId="509" priority="594">
       <formula>$AD41="Gráfico 15"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="518" priority="595">
+    <cfRule type="expression" dxfId="508" priority="595">
       <formula>$AD41="Gráfico 14"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="517" priority="596">
+    <cfRule type="expression" dxfId="507" priority="596">
       <formula>$AD41="Gráfico 12"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="516" priority="597">
+    <cfRule type="expression" dxfId="506" priority="597">
       <formula>$AD41="Gráfico 13"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="515" priority="598">
+    <cfRule type="expression" dxfId="505" priority="598">
       <formula>$AD41="Gráfico 11"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="514" priority="599">
+    <cfRule type="expression" dxfId="504" priority="599">
       <formula>$AD41="Gráfico 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="513" priority="600">
+    <cfRule type="expression" dxfId="503" priority="600">
       <formula>$AD41="Gráfico 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="512" priority="601">
+    <cfRule type="expression" dxfId="502" priority="601">
       <formula>$AD41="Gráfico 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="511" priority="602">
+    <cfRule type="expression" dxfId="501" priority="602">
       <formula>$AD41="Gráfico 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="510" priority="603">
+    <cfRule type="expression" dxfId="500" priority="603">
       <formula>$AD41="Gráfico 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="509" priority="604">
+    <cfRule type="expression" dxfId="499" priority="604">
       <formula>$AD41="Gráfico 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="508" priority="605">
+    <cfRule type="expression" dxfId="498" priority="605">
       <formula>$AD41="Gráfico 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="507" priority="606">
+    <cfRule type="expression" dxfId="497" priority="606">
       <formula>$AD41="Gráfico 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="506" priority="607">
+    <cfRule type="expression" dxfId="496" priority="607">
       <formula>$AD41="Gráfico 5"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N60:N62">
-    <cfRule type="expression" dxfId="505" priority="497">
+    <cfRule type="expression" dxfId="495" priority="497">
       <formula>$AE60="Reporte 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="504" priority="498">
+    <cfRule type="expression" dxfId="494" priority="498">
       <formula>$AE60="Reporte 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="503" priority="499">
+    <cfRule type="expression" dxfId="493" priority="499">
       <formula>$AE60="Informe 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="502" priority="500">
+    <cfRule type="expression" dxfId="492" priority="500">
       <formula>$AE60="Informe 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="501" priority="501">
+    <cfRule type="expression" dxfId="491" priority="501">
       <formula>$AE60="Informe 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="500" priority="502">
+    <cfRule type="expression" dxfId="490" priority="502">
       <formula>$AE60="Informe 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="499" priority="503">
+    <cfRule type="expression" dxfId="489" priority="503">
       <formula>$AE60="Informe 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="498" priority="504">
+    <cfRule type="expression" dxfId="488" priority="504">
       <formula>$AE60="Informe 5"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="497" priority="505">
+    <cfRule type="expression" dxfId="487" priority="505">
       <formula>$AE60="Informe 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="496" priority="506">
+    <cfRule type="expression" dxfId="486" priority="506">
       <formula>$AE60="Informe 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="495" priority="507">
+    <cfRule type="expression" dxfId="485" priority="507">
       <formula>$AE60="Informe 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="494" priority="508">
+    <cfRule type="expression" dxfId="484" priority="508">
       <formula>$AE60="Informe 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="493" priority="509">
+    <cfRule type="expression" dxfId="483" priority="509">
       <formula>$AE60="Gráfico 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="492" priority="510">
+    <cfRule type="expression" dxfId="482" priority="510">
       <formula>$AE60="Gráfico 25"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="491" priority="511">
+    <cfRule type="expression" dxfId="481" priority="511">
       <formula>$AE60="Gráfico 24"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="490" priority="512">
+    <cfRule type="expression" dxfId="480" priority="512">
       <formula>$AE60="Gráfico 23"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="489" priority="513">
+    <cfRule type="expression" dxfId="479" priority="513">
       <formula>$AE60="Gráfico 22"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="488" priority="514">
+    <cfRule type="expression" dxfId="478" priority="514">
       <formula>$AE60="Gráfico 21"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="487" priority="515">
+    <cfRule type="expression" dxfId="477" priority="515">
       <formula>$AE60="Gráfico 20"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="486" priority="516">
+    <cfRule type="expression" dxfId="476" priority="516">
       <formula>$AE60="Gráfico 18"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="485" priority="517">
+    <cfRule type="expression" dxfId="475" priority="517">
       <formula>$AE60="Gráfico 19"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="484" priority="518">
+    <cfRule type="expression" dxfId="474" priority="518">
       <formula>$AE60="Gráfico 17"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="483" priority="519">
+    <cfRule type="expression" dxfId="473" priority="519">
       <formula>$AE60="Gráfico 16"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="482" priority="520">
+    <cfRule type="expression" dxfId="472" priority="520">
       <formula>$AE60="Gráfico 15"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="481" priority="521">
+    <cfRule type="expression" dxfId="471" priority="521">
       <formula>$AE60="Gráfico 14"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="480" priority="522">
+    <cfRule type="expression" dxfId="470" priority="522">
       <formula>$AE60="Gráfico 12"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="479" priority="523">
+    <cfRule type="expression" dxfId="469" priority="523">
       <formula>$AE60="Gráfico 13"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="478" priority="524">
+    <cfRule type="expression" dxfId="468" priority="524">
       <formula>$AE60="Gráfico 11"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="477" priority="525">
+    <cfRule type="expression" dxfId="467" priority="525">
       <formula>$AE60="Gráfico 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="476" priority="526">
+    <cfRule type="expression" dxfId="466" priority="526">
       <formula>$AE60="Gráfico 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="475" priority="527">
+    <cfRule type="expression" dxfId="465" priority="527">
       <formula>$AE60="Gráfico 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="474" priority="528">
+    <cfRule type="expression" dxfId="464" priority="528">
       <formula>$AE60="Gráfico 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="473" priority="529">
+    <cfRule type="expression" dxfId="463" priority="529">
       <formula>$AE60="Gráfico 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="472" priority="530">
+    <cfRule type="expression" dxfId="462" priority="530">
       <formula>$AE60="Gráfico 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="471" priority="531">
+    <cfRule type="expression" dxfId="461" priority="531">
       <formula>$AE60="Gráfico 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="470" priority="532">
+    <cfRule type="expression" dxfId="460" priority="532">
       <formula>$AE60="Gráfico 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="469" priority="533">
+    <cfRule type="expression" dxfId="459" priority="533">
       <formula>$AE60="Gráfico 5"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N89:N91">
-    <cfRule type="expression" dxfId="468" priority="460">
+    <cfRule type="expression" dxfId="458" priority="460">
       <formula>$AD89="Reporte 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="467" priority="461">
+    <cfRule type="expression" dxfId="457" priority="461">
       <formula>$AD89="Reporte 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="466" priority="462">
+    <cfRule type="expression" dxfId="456" priority="462">
       <formula>$AD89="Informe 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="465" priority="463">
+    <cfRule type="expression" dxfId="455" priority="463">
       <formula>$AD89="Informe 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="464" priority="464">
+    <cfRule type="expression" dxfId="454" priority="464">
       <formula>$AD89="Informe 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="463" priority="465">
+    <cfRule type="expression" dxfId="453" priority="465">
       <formula>$AD89="Informe 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="462" priority="466">
+    <cfRule type="expression" dxfId="452" priority="466">
       <formula>$AD89="Informe 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="461" priority="467">
+    <cfRule type="expression" dxfId="451" priority="467">
       <formula>$AD89="Informe 5"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="460" priority="468">
+    <cfRule type="expression" dxfId="450" priority="468">
       <formula>$AD89="Informe 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="459" priority="469">
+    <cfRule type="expression" dxfId="449" priority="469">
       <formula>$AD89="Informe 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="458" priority="470">
+    <cfRule type="expression" dxfId="448" priority="470">
       <formula>$AD89="Informe 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="457" priority="471">
+    <cfRule type="expression" dxfId="447" priority="471">
       <formula>$AD89="Informe 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="456" priority="472">
+    <cfRule type="expression" dxfId="446" priority="472">
       <formula>$AD89="Gráfico 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="455" priority="473">
+    <cfRule type="expression" dxfId="445" priority="473">
       <formula>$AD89="Gráfico 25"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="454" priority="474">
+    <cfRule type="expression" dxfId="444" priority="474">
       <formula>$AD89="Gráfico 24"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="453" priority="475">
+    <cfRule type="expression" dxfId="443" priority="475">
       <formula>$AD89="Gráfico 23"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="452" priority="476">
+    <cfRule type="expression" dxfId="442" priority="476">
       <formula>$AD89="Gráfico 22"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="451" priority="477">
+    <cfRule type="expression" dxfId="441" priority="477">
       <formula>$AD89="Gráfico 21"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="450" priority="478">
+    <cfRule type="expression" dxfId="440" priority="478">
       <formula>$AD89="Gráfico 20"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="449" priority="479">
+    <cfRule type="expression" dxfId="439" priority="479">
       <formula>$AD89="Gráfico 18"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="448" priority="480">
+    <cfRule type="expression" dxfId="438" priority="480">
       <formula>$AD89="Gráfico 19"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="447" priority="481">
+    <cfRule type="expression" dxfId="437" priority="481">
       <formula>$AD89="Gráfico 17"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="446" priority="482">
+    <cfRule type="expression" dxfId="436" priority="482">
       <formula>$AD89="Gráfico 16"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="445" priority="483">
+    <cfRule type="expression" dxfId="435" priority="483">
       <formula>$AD89="Gráfico 15"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="444" priority="484">
+    <cfRule type="expression" dxfId="434" priority="484">
       <formula>$AD89="Gráfico 14"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="443" priority="485">
+    <cfRule type="expression" dxfId="433" priority="485">
       <formula>$AD89="Gráfico 12"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="442" priority="486">
+    <cfRule type="expression" dxfId="432" priority="486">
       <formula>$AD89="Gráfico 13"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="441" priority="487">
+    <cfRule type="expression" dxfId="431" priority="487">
       <formula>$AD89="Gráfico 11"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="440" priority="488">
+    <cfRule type="expression" dxfId="430" priority="488">
       <formula>$AD89="Gráfico 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="439" priority="489">
+    <cfRule type="expression" dxfId="429" priority="489">
       <formula>$AD89="Gráfico 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="438" priority="490">
+    <cfRule type="expression" dxfId="428" priority="490">
       <formula>$AD89="Gráfico 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="437" priority="491">
+    <cfRule type="expression" dxfId="427" priority="491">
       <formula>$AD89="Gráfico 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="436" priority="492">
+    <cfRule type="expression" dxfId="426" priority="492">
       <formula>$AD89="Gráfico 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="435" priority="493">
+    <cfRule type="expression" dxfId="425" priority="493">
       <formula>$AD89="Gráfico 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="434" priority="494">
+    <cfRule type="expression" dxfId="424" priority="494">
       <formula>$AD89="Gráfico 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="433" priority="495">
+    <cfRule type="expression" dxfId="423" priority="495">
       <formula>$AD89="Gráfico 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="432" priority="496">
+    <cfRule type="expression" dxfId="422" priority="496">
       <formula>$AD89="Gráfico 5"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N92:N94">
-    <cfRule type="expression" dxfId="431" priority="423">
+    <cfRule type="expression" dxfId="421" priority="423">
       <formula>$AD92="Reporte 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="430" priority="424">
+    <cfRule type="expression" dxfId="420" priority="424">
       <formula>$AD92="Reporte 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="429" priority="425">
+    <cfRule type="expression" dxfId="419" priority="425">
       <formula>$AD92="Informe 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="428" priority="426">
+    <cfRule type="expression" dxfId="418" priority="426">
       <formula>$AD92="Informe 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="427" priority="427">
+    <cfRule type="expression" dxfId="417" priority="427">
       <formula>$AD92="Informe 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="426" priority="428">
+    <cfRule type="expression" dxfId="416" priority="428">
       <formula>$AD92="Informe 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="425" priority="429">
+    <cfRule type="expression" dxfId="415" priority="429">
       <formula>$AD92="Informe 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="424" priority="430">
+    <cfRule type="expression" dxfId="414" priority="430">
       <formula>$AD92="Informe 5"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="423" priority="431">
+    <cfRule type="expression" dxfId="413" priority="431">
       <formula>$AD92="Informe 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="422" priority="432">
+    <cfRule type="expression" dxfId="412" priority="432">
       <formula>$AD92="Informe 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="421" priority="433">
+    <cfRule type="expression" dxfId="411" priority="433">
       <formula>$AD92="Informe 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="420" priority="434">
+    <cfRule type="expression" dxfId="410" priority="434">
       <formula>$AD92="Informe 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="419" priority="435">
+    <cfRule type="expression" dxfId="409" priority="435">
       <formula>$AD92="Gráfico 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="418" priority="436">
+    <cfRule type="expression" dxfId="408" priority="436">
       <formula>$AD92="Gráfico 25"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="417" priority="437">
+    <cfRule type="expression" dxfId="407" priority="437">
       <formula>$AD92="Gráfico 24"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="416" priority="438">
+    <cfRule type="expression" dxfId="406" priority="438">
       <formula>$AD92="Gráfico 23"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="415" priority="439">
+    <cfRule type="expression" dxfId="405" priority="439">
       <formula>$AD92="Gráfico 22"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="414" priority="440">
+    <cfRule type="expression" dxfId="404" priority="440">
       <formula>$AD92="Gráfico 21"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="413" priority="441">
+    <cfRule type="expression" dxfId="403" priority="441">
       <formula>$AD92="Gráfico 20"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="412" priority="442">
+    <cfRule type="expression" dxfId="402" priority="442">
       <formula>$AD92="Gráfico 18"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="411" priority="443">
+    <cfRule type="expression" dxfId="401" priority="443">
       <formula>$AD92="Gráfico 19"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="410" priority="444">
+    <cfRule type="expression" dxfId="400" priority="444">
       <formula>$AD92="Gráfico 17"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="409" priority="445">
+    <cfRule type="expression" dxfId="399" priority="445">
       <formula>$AD92="Gráfico 16"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="408" priority="446">
+    <cfRule type="expression" dxfId="398" priority="446">
       <formula>$AD92="Gráfico 15"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="407" priority="447">
+    <cfRule type="expression" dxfId="397" priority="447">
       <formula>$AD92="Gráfico 14"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="406" priority="448">
+    <cfRule type="expression" dxfId="396" priority="448">
       <formula>$AD92="Gráfico 12"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="405" priority="449">
+    <cfRule type="expression" dxfId="395" priority="449">
       <formula>$AD92="Gráfico 13"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="404" priority="450">
+    <cfRule type="expression" dxfId="394" priority="450">
       <formula>$AD92="Gráfico 11"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="403" priority="451">
+    <cfRule type="expression" dxfId="393" priority="451">
       <formula>$AD92="Gráfico 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="402" priority="452">
+    <cfRule type="expression" dxfId="392" priority="452">
       <formula>$AD92="Gráfico 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="401" priority="453">
+    <cfRule type="expression" dxfId="391" priority="453">
       <formula>$AD92="Gráfico 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="400" priority="454">
+    <cfRule type="expression" dxfId="390" priority="454">
       <formula>$AD92="Gráfico 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="399" priority="455">
+    <cfRule type="expression" dxfId="389" priority="455">
       <formula>$AD92="Gráfico 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="398" priority="456">
+    <cfRule type="expression" dxfId="388" priority="456">
       <formula>$AD92="Gráfico 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="397" priority="457">
+    <cfRule type="expression" dxfId="387" priority="457">
       <formula>$AD92="Gráfico 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="396" priority="458">
+    <cfRule type="expression" dxfId="386" priority="458">
       <formula>$AD92="Gráfico 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="395" priority="459">
+    <cfRule type="expression" dxfId="385" priority="459">
       <formula>$AD92="Gráfico 5"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M48">
-    <cfRule type="expression" dxfId="394" priority="386">
+    <cfRule type="expression" dxfId="384" priority="386">
       <formula>#REF!="Reporte 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="393" priority="387">
+    <cfRule type="expression" dxfId="383" priority="387">
       <formula>#REF!="Reporte 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="392" priority="388">
+    <cfRule type="expression" dxfId="382" priority="388">
       <formula>#REF!="Informe 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="391" priority="389">
+    <cfRule type="expression" dxfId="381" priority="389">
       <formula>#REF!="Informe 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="390" priority="390">
+    <cfRule type="expression" dxfId="380" priority="390">
       <formula>#REF!="Informe 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="389" priority="391">
+    <cfRule type="expression" dxfId="379" priority="391">
       <formula>#REF!="Informe 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="388" priority="392">
+    <cfRule type="expression" dxfId="378" priority="392">
       <formula>#REF!="Informe 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="387" priority="393">
+    <cfRule type="expression" dxfId="377" priority="393">
       <formula>#REF!="Informe 5"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="386" priority="394">
+    <cfRule type="expression" dxfId="376" priority="394">
       <formula>#REF!="Informe 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="385" priority="395">
+    <cfRule type="expression" dxfId="375" priority="395">
       <formula>#REF!="Informe 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="384" priority="396">
+    <cfRule type="expression" dxfId="374" priority="396">
       <formula>#REF!="Informe 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="383" priority="397">
+    <cfRule type="expression" dxfId="373" priority="397">
       <formula>#REF!="Informe 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="382" priority="398">
+    <cfRule type="expression" dxfId="372" priority="398">
       <formula>#REF!="Gráfico 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="381" priority="399">
+    <cfRule type="expression" dxfId="371" priority="399">
       <formula>#REF!="Gráfico 25"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="380" priority="400">
+    <cfRule type="expression" dxfId="370" priority="400">
       <formula>#REF!="Gráfico 24"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="379" priority="401">
+    <cfRule type="expression" dxfId="369" priority="401">
       <formula>#REF!="Gráfico 23"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="378" priority="402">
+    <cfRule type="expression" dxfId="368" priority="402">
       <formula>#REF!="Gráfico 22"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="377" priority="403">
+    <cfRule type="expression" dxfId="367" priority="403">
       <formula>#REF!="Gráfico 21"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="376" priority="404">
+    <cfRule type="expression" dxfId="366" priority="404">
       <formula>#REF!="Gráfico 20"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="375" priority="405">
+    <cfRule type="expression" dxfId="365" priority="405">
       <formula>#REF!="Gráfico 18"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="374" priority="406">
+    <cfRule type="expression" dxfId="364" priority="406">
       <formula>#REF!="Gráfico 19"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="373" priority="407">
+    <cfRule type="expression" dxfId="363" priority="407">
       <formula>#REF!="Gráfico 17"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="372" priority="408">
+    <cfRule type="expression" dxfId="362" priority="408">
       <formula>#REF!="Gráfico 16"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="371" priority="409">
+    <cfRule type="expression" dxfId="361" priority="409">
       <formula>#REF!="Gráfico 15"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="370" priority="410">
+    <cfRule type="expression" dxfId="360" priority="410">
       <formula>#REF!="Gráfico 14"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="369" priority="411">
+    <cfRule type="expression" dxfId="359" priority="411">
       <formula>#REF!="Gráfico 12"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="368" priority="412">
+    <cfRule type="expression" dxfId="358" priority="412">
       <formula>#REF!="Gráfico 13"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="367" priority="413">
+    <cfRule type="expression" dxfId="357" priority="413">
       <formula>#REF!="Gráfico 11"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="366" priority="414">
+    <cfRule type="expression" dxfId="356" priority="414">
       <formula>#REF!="Gráfico 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="365" priority="415">
+    <cfRule type="expression" dxfId="355" priority="415">
       <formula>#REF!="Gráfico 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="364" priority="416">
+    <cfRule type="expression" dxfId="354" priority="416">
       <formula>#REF!="Gráfico 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="363" priority="417">
+    <cfRule type="expression" dxfId="353" priority="417">
       <formula>#REF!="Gráfico 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="362" priority="418">
+    <cfRule type="expression" dxfId="352" priority="418">
       <formula>#REF!="Gráfico 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="361" priority="419">
+    <cfRule type="expression" dxfId="351" priority="419">
       <formula>#REF!="Gráfico 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="360" priority="420">
+    <cfRule type="expression" dxfId="350" priority="420">
       <formula>#REF!="Gráfico 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="359" priority="421">
+    <cfRule type="expression" dxfId="349" priority="421">
       <formula>#REF!="Gráfico 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="358" priority="422">
+    <cfRule type="expression" dxfId="348" priority="422">
       <formula>#REF!="Gráfico 5"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L48">
-    <cfRule type="expression" dxfId="357" priority="349">
+    <cfRule type="expression" dxfId="347" priority="349">
       <formula>#REF!="Reporte 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="356" priority="350">
+    <cfRule type="expression" dxfId="346" priority="350">
       <formula>#REF!="Reporte 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="355" priority="351">
+    <cfRule type="expression" dxfId="345" priority="351">
       <formula>#REF!="Informe 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="354" priority="352">
+    <cfRule type="expression" dxfId="344" priority="352">
       <formula>#REF!="Informe 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="353" priority="353">
+    <cfRule type="expression" dxfId="343" priority="353">
       <formula>#REF!="Informe 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="352" priority="354">
+    <cfRule type="expression" dxfId="342" priority="354">
       <formula>#REF!="Informe 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="351" priority="355">
+    <cfRule type="expression" dxfId="341" priority="355">
       <formula>#REF!="Informe 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="350" priority="356">
+    <cfRule type="expression" dxfId="340" priority="356">
       <formula>#REF!="Informe 5"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="349" priority="357">
+    <cfRule type="expression" dxfId="339" priority="357">
       <formula>#REF!="Informe 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="348" priority="358">
+    <cfRule type="expression" dxfId="338" priority="358">
       <formula>#REF!="Informe 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="347" priority="359">
+    <cfRule type="expression" dxfId="337" priority="359">
       <formula>#REF!="Informe 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="346" priority="360">
+    <cfRule type="expression" dxfId="336" priority="360">
       <formula>#REF!="Informe 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="345" priority="361">
+    <cfRule type="expression" dxfId="335" priority="361">
       <formula>#REF!="Gráfico 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="344" priority="362">
+    <cfRule type="expression" dxfId="334" priority="362">
       <formula>#REF!="Gráfico 25"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="343" priority="363">
+    <cfRule type="expression" dxfId="333" priority="363">
       <formula>#REF!="Gráfico 24"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="342" priority="364">
+    <cfRule type="expression" dxfId="332" priority="364">
       <formula>#REF!="Gráfico 23"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="341" priority="365">
+    <cfRule type="expression" dxfId="331" priority="365">
       <formula>#REF!="Gráfico 22"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="340" priority="366">
+    <cfRule type="expression" dxfId="330" priority="366">
       <formula>#REF!="Gráfico 21"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="339" priority="367">
+    <cfRule type="expression" dxfId="329" priority="367">
       <formula>#REF!="Gráfico 20"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="338" priority="368">
+    <cfRule type="expression" dxfId="328" priority="368">
       <formula>#REF!="Gráfico 18"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="337" priority="369">
+    <cfRule type="expression" dxfId="327" priority="369">
       <formula>#REF!="Gráfico 19"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="336" priority="370">
+    <cfRule type="expression" dxfId="326" priority="370">
       <formula>#REF!="Gráfico 17"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="335" priority="371">
+    <cfRule type="expression" dxfId="325" priority="371">
       <formula>#REF!="Gráfico 16"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="334" priority="372">
+    <cfRule type="expression" dxfId="324" priority="372">
       <formula>#REF!="Gráfico 15"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="333" priority="373">
+    <cfRule type="expression" dxfId="323" priority="373">
       <formula>#REF!="Gráfico 14"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="332" priority="374">
+    <cfRule type="expression" dxfId="322" priority="374">
       <formula>#REF!="Gráfico 12"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="331" priority="375">
+    <cfRule type="expression" dxfId="321" priority="375">
       <formula>#REF!="Gráfico 13"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="330" priority="376">
+    <cfRule type="expression" dxfId="320" priority="376">
       <formula>#REF!="Gráfico 11"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="329" priority="377">
+    <cfRule type="expression" dxfId="319" priority="377">
       <formula>#REF!="Gráfico 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="328" priority="378">
+    <cfRule type="expression" dxfId="318" priority="378">
       <formula>#REF!="Gráfico 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="327" priority="379">
+    <cfRule type="expression" dxfId="317" priority="379">
       <formula>#REF!="Gráfico 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="326" priority="380">
+    <cfRule type="expression" dxfId="316" priority="380">
       <formula>#REF!="Gráfico 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="325" priority="381">
+    <cfRule type="expression" dxfId="315" priority="381">
       <formula>#REF!="Gráfico 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="324" priority="382">
+    <cfRule type="expression" dxfId="314" priority="382">
       <formula>#REF!="Gráfico 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="323" priority="383">
+    <cfRule type="expression" dxfId="313" priority="383">
       <formula>#REF!="Gráfico 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="322" priority="384">
+    <cfRule type="expression" dxfId="312" priority="384">
       <formula>#REF!="Gráfico 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="321" priority="385">
+    <cfRule type="expression" dxfId="311" priority="385">
       <formula>#REF!="Gráfico 5"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11:K96">
-    <cfRule type="containsText" dxfId="320" priority="113" operator="containsText" text="cambiado">
+    <cfRule type="containsText" dxfId="310" priority="113" operator="containsText" text="cambiado">
       <formula>NOT(ISERROR(SEARCH("cambiado",K11)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="319" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="309" priority="114" operator="equal">
       <formula>"revisar"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="318" priority="347" operator="equal">
+    <cfRule type="cellIs" dxfId="308" priority="347" operator="equal">
       <formula>"pendiente"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="317" priority="348" operator="equal">
+    <cfRule type="cellIs" dxfId="307" priority="348" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E69:E71 E75:E94 E11:E65">
-    <cfRule type="cellIs" dxfId="316" priority="344" operator="equal">
+    <cfRule type="cellIs" dxfId="306" priority="344" operator="equal">
       <formula>"pendiente"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="315" priority="345" operator="equal">
+    <cfRule type="cellIs" dxfId="305" priority="345" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="314" priority="346" operator="equal">
+    <cfRule type="cellIs" dxfId="304" priority="346" operator="equal">
       <formula>"en proceso"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L62:M62">
-    <cfRule type="expression" dxfId="313" priority="233">
+    <cfRule type="expression" dxfId="303" priority="233">
       <formula>$AA62="Reporte 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="312" priority="234">
+    <cfRule type="expression" dxfId="302" priority="234">
       <formula>$AA62="Reporte 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="311" priority="235">
+    <cfRule type="expression" dxfId="301" priority="235">
       <formula>$AA62="Informe 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="310" priority="236">
+    <cfRule type="expression" dxfId="300" priority="236">
       <formula>$AA62="Informe 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="309" priority="237">
+    <cfRule type="expression" dxfId="299" priority="237">
       <formula>$AA62="Informe 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="308" priority="238">
+    <cfRule type="expression" dxfId="298" priority="238">
       <formula>$AA62="Informe 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="307" priority="239">
+    <cfRule type="expression" dxfId="297" priority="239">
       <formula>$AA62="Informe 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="306" priority="240">
+    <cfRule type="expression" dxfId="296" priority="240">
       <formula>$AA62="Informe 5"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="305" priority="241">
+    <cfRule type="expression" dxfId="295" priority="241">
       <formula>$AA62="Informe 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="304" priority="242">
+    <cfRule type="expression" dxfId="294" priority="242">
       <formula>$AA62="Informe 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="303" priority="243">
+    <cfRule type="expression" dxfId="293" priority="243">
       <formula>$AA62="Informe 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="302" priority="244">
+    <cfRule type="expression" dxfId="292" priority="244">
       <formula>$AA62="Informe 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="301" priority="245">
+    <cfRule type="expression" dxfId="291" priority="245">
       <formula>$AA62="Gráfico 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="300" priority="246">
+    <cfRule type="expression" dxfId="290" priority="246">
       <formula>$AA62="Gráfico 25"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="299" priority="247">
+    <cfRule type="expression" dxfId="289" priority="247">
       <formula>$AA62="Gráfico 24"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="298" priority="248">
+    <cfRule type="expression" dxfId="288" priority="248">
       <formula>$AA62="Gráfico 23"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="297" priority="249">
+    <cfRule type="expression" dxfId="287" priority="249">
       <formula>$AA62="Gráfico 22"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="296" priority="250">
+    <cfRule type="expression" dxfId="286" priority="250">
       <formula>$AA62="Gráfico 21"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="295" priority="251">
+    <cfRule type="expression" dxfId="285" priority="251">
       <formula>$AA62="Gráfico 20"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="294" priority="252">
+    <cfRule type="expression" dxfId="284" priority="252">
       <formula>$AA62="Gráfico 18"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="293" priority="253">
+    <cfRule type="expression" dxfId="283" priority="253">
       <formula>$AA62="Gráfico 19"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="292" priority="254">
+    <cfRule type="expression" dxfId="282" priority="254">
       <formula>$AA62="Gráfico 17"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="291" priority="255">
+    <cfRule type="expression" dxfId="281" priority="255">
       <formula>$AA62="Gráfico 16"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="290" priority="256">
+    <cfRule type="expression" dxfId="280" priority="256">
       <formula>$AA62="Gráfico 15"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="289" priority="257">
+    <cfRule type="expression" dxfId="279" priority="257">
       <formula>$AA62="Gráfico 14"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="288" priority="258">
+    <cfRule type="expression" dxfId="278" priority="258">
       <formula>$AA62="Gráfico 12"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="287" priority="259">
+    <cfRule type="expression" dxfId="277" priority="259">
       <formula>$AA62="Gráfico 13"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="286" priority="260">
+    <cfRule type="expression" dxfId="276" priority="260">
       <formula>$AA62="Gráfico 11"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="285" priority="261">
+    <cfRule type="expression" dxfId="275" priority="261">
       <formula>$AA62="Gráfico 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="284" priority="262">
+    <cfRule type="expression" dxfId="274" priority="262">
       <formula>$AA62="Gráfico 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="283" priority="263">
+    <cfRule type="expression" dxfId="273" priority="263">
       <formula>$AA62="Gráfico 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="282" priority="264">
+    <cfRule type="expression" dxfId="272" priority="264">
       <formula>$AA62="Gráfico 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="281" priority="265">
+    <cfRule type="expression" dxfId="271" priority="265">
       <formula>$AA62="Gráfico 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="280" priority="266">
+    <cfRule type="expression" dxfId="270" priority="266">
       <formula>$AA62="Gráfico 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="279" priority="267">
+    <cfRule type="expression" dxfId="269" priority="267">
       <formula>$AA62="Gráfico 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="278" priority="268">
+    <cfRule type="expression" dxfId="268" priority="268">
       <formula>$AA62="Gráfico 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="277" priority="269">
+    <cfRule type="expression" dxfId="267" priority="269">
       <formula>$AA62="Gráfico 5"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L60:M60">
-    <cfRule type="expression" dxfId="276" priority="270">
+    <cfRule type="expression" dxfId="266" priority="270">
       <formula>$AA62="Reporte 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="275" priority="271">
+    <cfRule type="expression" dxfId="265" priority="271">
       <formula>$AA62="Reporte 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="274" priority="272">
+    <cfRule type="expression" dxfId="264" priority="272">
       <formula>$AA62="Informe 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="273" priority="273">
+    <cfRule type="expression" dxfId="263" priority="273">
       <formula>$AA62="Informe 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="272" priority="274">
+    <cfRule type="expression" dxfId="262" priority="274">
       <formula>$AA62="Informe 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="271" priority="275">
+    <cfRule type="expression" dxfId="261" priority="275">
       <formula>$AA62="Informe 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="270" priority="276">
+    <cfRule type="expression" dxfId="260" priority="276">
       <formula>$AA62="Informe 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="269" priority="277">
+    <cfRule type="expression" dxfId="259" priority="277">
       <formula>$AA62="Informe 5"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="268" priority="278">
+    <cfRule type="expression" dxfId="258" priority="278">
       <formula>$AA62="Informe 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="267" priority="279">
+    <cfRule type="expression" dxfId="257" priority="279">
       <formula>$AA62="Informe 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="266" priority="280">
+    <cfRule type="expression" dxfId="256" priority="280">
       <formula>$AA62="Informe 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="265" priority="281">
+    <cfRule type="expression" dxfId="255" priority="281">
       <formula>$AA62="Informe 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="264" priority="282">
+    <cfRule type="expression" dxfId="254" priority="282">
       <formula>$AA62="Gráfico 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="263" priority="283">
+    <cfRule type="expression" dxfId="253" priority="283">
       <formula>$AA62="Gráfico 25"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="262" priority="284">
+    <cfRule type="expression" dxfId="252" priority="284">
       <formula>$AA62="Gráfico 24"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="261" priority="285">
+    <cfRule type="expression" dxfId="251" priority="285">
       <formula>$AA62="Gráfico 23"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="260" priority="286">
+    <cfRule type="expression" dxfId="250" priority="286">
       <formula>$AA62="Gráfico 22"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="259" priority="287">
+    <cfRule type="expression" dxfId="249" priority="287">
       <formula>$AA62="Gráfico 21"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="258" priority="288">
+    <cfRule type="expression" dxfId="248" priority="288">
       <formula>$AA62="Gráfico 20"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="257" priority="289">
+    <cfRule type="expression" dxfId="247" priority="289">
       <formula>$AA62="Gráfico 18"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="256" priority="290">
+    <cfRule type="expression" dxfId="246" priority="290">
       <formula>$AA62="Gráfico 19"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="255" priority="291">
+    <cfRule type="expression" dxfId="245" priority="291">
       <formula>$AA62="Gráfico 17"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="254" priority="292">
+    <cfRule type="expression" dxfId="244" priority="292">
       <formula>$AA62="Gráfico 16"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="253" priority="293">
+    <cfRule type="expression" dxfId="243" priority="293">
       <formula>$AA62="Gráfico 15"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="252" priority="294">
+    <cfRule type="expression" dxfId="242" priority="294">
       <formula>$AA62="Gráfico 14"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="251" priority="295">
+    <cfRule type="expression" dxfId="241" priority="295">
       <formula>$AA62="Gráfico 12"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="250" priority="296">
+    <cfRule type="expression" dxfId="240" priority="296">
       <formula>$AA62="Gráfico 13"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="249" priority="297">
+    <cfRule type="expression" dxfId="239" priority="297">
       <formula>$AA62="Gráfico 11"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="248" priority="298">
+    <cfRule type="expression" dxfId="238" priority="298">
       <formula>$AA62="Gráfico 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="247" priority="299">
+    <cfRule type="expression" dxfId="237" priority="299">
       <formula>$AA62="Gráfico 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="246" priority="300">
+    <cfRule type="expression" dxfId="236" priority="300">
       <formula>$AA62="Gráfico 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="245" priority="301">
+    <cfRule type="expression" dxfId="235" priority="301">
       <formula>$AA62="Gráfico 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="244" priority="302">
+    <cfRule type="expression" dxfId="234" priority="302">
       <formula>$AA62="Gráfico 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="243" priority="303">
+    <cfRule type="expression" dxfId="233" priority="303">
       <formula>$AA62="Gráfico 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="242" priority="304">
+    <cfRule type="expression" dxfId="232" priority="304">
       <formula>$AA62="Gráfico 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="241" priority="305">
+    <cfRule type="expression" dxfId="231" priority="305">
       <formula>$AA62="Gráfico 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="240" priority="306">
+    <cfRule type="expression" dxfId="230" priority="306">
       <formula>$AA62="Gráfico 5"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M60">
-    <cfRule type="expression" dxfId="239" priority="196">
+    <cfRule type="expression" dxfId="229" priority="196">
       <formula>$AA62="Reporte 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="238" priority="197">
+    <cfRule type="expression" dxfId="228" priority="197">
       <formula>$AA62="Reporte 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="237" priority="198">
+    <cfRule type="expression" dxfId="227" priority="198">
       <formula>$AA62="Informe 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="236" priority="199">
+    <cfRule type="expression" dxfId="226" priority="199">
       <formula>$AA62="Informe 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="235" priority="200">
+    <cfRule type="expression" dxfId="225" priority="200">
       <formula>$AA62="Informe 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="234" priority="201">
+    <cfRule type="expression" dxfId="224" priority="201">
       <formula>$AA62="Informe 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="233" priority="202">
+    <cfRule type="expression" dxfId="223" priority="202">
       <formula>$AA62="Informe 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="232" priority="203">
+    <cfRule type="expression" dxfId="222" priority="203">
       <formula>$AA62="Informe 5"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="231" priority="204">
+    <cfRule type="expression" dxfId="221" priority="204">
       <formula>$AA62="Informe 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="230" priority="205">
+    <cfRule type="expression" dxfId="220" priority="205">
       <formula>$AA62="Informe 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="229" priority="206">
+    <cfRule type="expression" dxfId="219" priority="206">
       <formula>$AA62="Informe 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="228" priority="207">
+    <cfRule type="expression" dxfId="218" priority="207">
       <formula>$AA62="Informe 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="227" priority="208">
+    <cfRule type="expression" dxfId="217" priority="208">
       <formula>$AA62="Gráfico 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="226" priority="209">
+    <cfRule type="expression" dxfId="216" priority="209">
       <formula>$AA62="Gráfico 25"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="225" priority="210">
+    <cfRule type="expression" dxfId="215" priority="210">
       <formula>$AA62="Gráfico 24"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="224" priority="211">
+    <cfRule type="expression" dxfId="214" priority="211">
       <formula>$AA62="Gráfico 23"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="223" priority="212">
+    <cfRule type="expression" dxfId="213" priority="212">
       <formula>$AA62="Gráfico 22"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="222" priority="213">
+    <cfRule type="expression" dxfId="212" priority="213">
       <formula>$AA62="Gráfico 21"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="221" priority="214">
+    <cfRule type="expression" dxfId="211" priority="214">
       <formula>$AA62="Gráfico 20"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="220" priority="215">
+    <cfRule type="expression" dxfId="210" priority="215">
       <formula>$AA62="Gráfico 18"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="219" priority="216">
+    <cfRule type="expression" dxfId="209" priority="216">
       <formula>$AA62="Gráfico 19"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="218" priority="217">
+    <cfRule type="expression" dxfId="208" priority="217">
       <formula>$AA62="Gráfico 17"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="217" priority="218">
+    <cfRule type="expression" dxfId="207" priority="218">
       <formula>$AA62="Gráfico 16"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="216" priority="219">
+    <cfRule type="expression" dxfId="206" priority="219">
       <formula>$AA62="Gráfico 15"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="215" priority="220">
+    <cfRule type="expression" dxfId="205" priority="220">
       <formula>$AA62="Gráfico 14"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="214" priority="221">
+    <cfRule type="expression" dxfId="204" priority="221">
       <formula>$AA62="Gráfico 12"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="213" priority="222">
+    <cfRule type="expression" dxfId="203" priority="222">
       <formula>$AA62="Gráfico 13"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="212" priority="223">
+    <cfRule type="expression" dxfId="202" priority="223">
       <formula>$AA62="Gráfico 11"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="211" priority="224">
+    <cfRule type="expression" dxfId="201" priority="224">
       <formula>$AA62="Gráfico 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="210" priority="225">
+    <cfRule type="expression" dxfId="200" priority="225">
       <formula>$AA62="Gráfico 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="209" priority="226">
+    <cfRule type="expression" dxfId="199" priority="226">
       <formula>$AA62="Gráfico 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="208" priority="227">
+    <cfRule type="expression" dxfId="198" priority="227">
       <formula>$AA62="Gráfico 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="207" priority="228">
+    <cfRule type="expression" dxfId="197" priority="228">
       <formula>$AA62="Gráfico 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="206" priority="229">
+    <cfRule type="expression" dxfId="196" priority="229">
       <formula>$AA62="Gráfico 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="205" priority="230">
+    <cfRule type="expression" dxfId="195" priority="230">
       <formula>$AA62="Gráfico 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="204" priority="231">
+    <cfRule type="expression" dxfId="194" priority="231">
       <formula>$AA62="Gráfico 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="203" priority="232">
+    <cfRule type="expression" dxfId="193" priority="232">
       <formula>$AA62="Gráfico 5"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L61:M61">
-    <cfRule type="expression" dxfId="202" priority="1107">
+    <cfRule type="expression" dxfId="192" priority="1107">
       <formula>#REF!="Reporte 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="201" priority="1108">
+    <cfRule type="expression" dxfId="191" priority="1108">
       <formula>#REF!="Reporte 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="200" priority="1109">
+    <cfRule type="expression" dxfId="190" priority="1109">
       <formula>#REF!="Informe 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="199" priority="1110">
+    <cfRule type="expression" dxfId="189" priority="1110">
       <formula>#REF!="Informe 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="198" priority="1111">
+    <cfRule type="expression" dxfId="188" priority="1111">
       <formula>#REF!="Informe 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="197" priority="1112">
+    <cfRule type="expression" dxfId="187" priority="1112">
       <formula>#REF!="Informe 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="196" priority="1113">
+    <cfRule type="expression" dxfId="186" priority="1113">
       <formula>#REF!="Informe 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="195" priority="1114">
+    <cfRule type="expression" dxfId="185" priority="1114">
       <formula>#REF!="Informe 5"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="194" priority="1115">
+    <cfRule type="expression" dxfId="184" priority="1115">
       <formula>#REF!="Informe 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="193" priority="1116">
+    <cfRule type="expression" dxfId="183" priority="1116">
       <formula>#REF!="Informe 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="192" priority="1117">
+    <cfRule type="expression" dxfId="182" priority="1117">
       <formula>#REF!="Informe 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="191" priority="1118">
+    <cfRule type="expression" dxfId="181" priority="1118">
       <formula>#REF!="Informe 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="190" priority="1119">
+    <cfRule type="expression" dxfId="180" priority="1119">
       <formula>#REF!="Gráfico 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="189" priority="1120">
+    <cfRule type="expression" dxfId="179" priority="1120">
       <formula>#REF!="Gráfico 25"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="188" priority="1121">
+    <cfRule type="expression" dxfId="178" priority="1121">
       <formula>#REF!="Gráfico 24"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O60:O62">
-    <cfRule type="expression" dxfId="187" priority="159">
+    <cfRule type="expression" dxfId="177" priority="159">
       <formula>$AA60="Reporte 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="186" priority="160">
+    <cfRule type="expression" dxfId="176" priority="160">
       <formula>$AA60="Reporte 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="185" priority="161">
+    <cfRule type="expression" dxfId="175" priority="161">
       <formula>$AA60="Informe 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="184" priority="162">
+    <cfRule type="expression" dxfId="174" priority="162">
       <formula>$AA60="Informe 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="183" priority="163">
+    <cfRule type="expression" dxfId="173" priority="163">
       <formula>$AA60="Informe 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="182" priority="164">
+    <cfRule type="expression" dxfId="172" priority="164">
       <formula>$AA60="Informe 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="181" priority="165">
+    <cfRule type="expression" dxfId="171" priority="165">
       <formula>$AA60="Informe 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="180" priority="166">
+    <cfRule type="expression" dxfId="170" priority="166">
       <formula>$AA60="Informe 5"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="179" priority="167">
+    <cfRule type="expression" dxfId="169" priority="167">
       <formula>$AA60="Informe 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="178" priority="168">
+    <cfRule type="expression" dxfId="168" priority="168">
       <formula>$AA60="Informe 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="177" priority="169">
+    <cfRule type="expression" dxfId="167" priority="169">
       <formula>$AA60="Informe 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="176" priority="170">
+    <cfRule type="expression" dxfId="166" priority="170">
       <formula>$AA60="Informe 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="175" priority="171">
+    <cfRule type="expression" dxfId="165" priority="171">
       <formula>$AA60="Gráfico 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="174" priority="172">
+    <cfRule type="expression" dxfId="164" priority="172">
       <formula>$AA60="Gráfico 25"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="173" priority="173">
+    <cfRule type="expression" dxfId="163" priority="173">
       <formula>$AA60="Gráfico 24"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="172" priority="174">
+    <cfRule type="expression" dxfId="162" priority="174">
       <formula>$AA60="Gráfico 23"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="171" priority="175">
+    <cfRule type="expression" dxfId="161" priority="175">
       <formula>$AA60="Gráfico 22"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="170" priority="176">
+    <cfRule type="expression" dxfId="160" priority="176">
       <formula>$AA60="Gráfico 21"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="169" priority="177">
+    <cfRule type="expression" dxfId="159" priority="177">
       <formula>$AA60="Gráfico 20"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="168" priority="178">
+    <cfRule type="expression" dxfId="158" priority="178">
       <formula>$AA60="Gráfico 18"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="167" priority="179">
+    <cfRule type="expression" dxfId="157" priority="179">
       <formula>$AA60="Gráfico 19"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="166" priority="180">
+    <cfRule type="expression" dxfId="156" priority="180">
       <formula>$AA60="Gráfico 17"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="165" priority="181">
+    <cfRule type="expression" dxfId="155" priority="181">
       <formula>$AA60="Gráfico 16"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="164" priority="182">
+    <cfRule type="expression" dxfId="154" priority="182">
       <formula>$AA60="Gráfico 15"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="163" priority="183">
+    <cfRule type="expression" dxfId="153" priority="183">
       <formula>$AA60="Gráfico 14"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="162" priority="184">
+    <cfRule type="expression" dxfId="152" priority="184">
       <formula>$AA60="Gráfico 12"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="161" priority="185">
+    <cfRule type="expression" dxfId="151" priority="185">
       <formula>$AA60="Gráfico 13"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="160" priority="186">
+    <cfRule type="expression" dxfId="150" priority="186">
       <formula>$AA60="Gráfico 11"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="159" priority="187">
+    <cfRule type="expression" dxfId="149" priority="187">
       <formula>$AA60="Gráfico 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="158" priority="188">
+    <cfRule type="expression" dxfId="148" priority="188">
       <formula>$AA60="Gráfico 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="157" priority="189">
+    <cfRule type="expression" dxfId="147" priority="189">
       <formula>$AA60="Gráfico 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="156" priority="190">
+    <cfRule type="expression" dxfId="146" priority="190">
       <formula>$AA60="Gráfico 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="155" priority="191">
+    <cfRule type="expression" dxfId="145" priority="191">
       <formula>$AA60="Gráfico 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="154" priority="192">
+    <cfRule type="expression" dxfId="144" priority="192">
       <formula>$AA60="Gráfico 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="153" priority="193">
+    <cfRule type="expression" dxfId="143" priority="193">
       <formula>$AA60="Gráfico 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="152" priority="194">
+    <cfRule type="expression" dxfId="142" priority="194">
       <formula>$AA60="Gráfico 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="151" priority="195">
+    <cfRule type="expression" dxfId="141" priority="195">
       <formula>$AA60="Gráfico 5"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66:E68">
-    <cfRule type="cellIs" dxfId="150" priority="156" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="156" operator="equal">
       <formula>"pendiente"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="157" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="157" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="158" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="158" operator="equal">
       <formula>"en proceso"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E72:E74">
-    <cfRule type="cellIs" dxfId="147" priority="153" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="153" operator="equal">
       <formula>"pendiente"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="154" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="154" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="155" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="155" operator="equal">
       <formula>"en proceso"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L45:L47">
-    <cfRule type="expression" dxfId="144" priority="121" stopIfTrue="1">
+    <cfRule type="expression" dxfId="134" priority="121" stopIfTrue="1">
       <formula>#REF!="Informe 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="143" priority="125" stopIfTrue="1">
+    <cfRule type="expression" dxfId="133" priority="125" stopIfTrue="1">
       <formula>#REF!="Informe 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="142" priority="152">
+    <cfRule type="expression" dxfId="132" priority="152">
       <formula>#REF!="Gráfico 5"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O21:O32">
-    <cfRule type="expression" dxfId="141" priority="76">
+    <cfRule type="expression" dxfId="131" priority="76">
       <formula>$Y21="Reporte 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="140" priority="77">
+    <cfRule type="expression" dxfId="130" priority="77">
       <formula>$Y21="Reporte 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="139" priority="78">
+    <cfRule type="expression" dxfId="129" priority="78">
       <formula>$Y21="Informe 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="138" priority="79">
+    <cfRule type="expression" dxfId="128" priority="79">
       <formula>$Y21="Informe 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="137" priority="80">
+    <cfRule type="expression" dxfId="127" priority="80">
       <formula>$Y21="Informe 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="136" priority="81">
+    <cfRule type="expression" dxfId="126" priority="81">
       <formula>$Y21="Informe 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="135" priority="82">
+    <cfRule type="expression" dxfId="125" priority="82">
       <formula>$Y21="Informe 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="134" priority="83">
+    <cfRule type="expression" dxfId="124" priority="83">
       <formula>$Y21="Informe 5"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="133" priority="84">
+    <cfRule type="expression" dxfId="123" priority="84">
       <formula>$Y21="Informe 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="132" priority="85">
+    <cfRule type="expression" dxfId="122" priority="85">
       <formula>$Y21="Informe 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="131" priority="86">
+    <cfRule type="expression" dxfId="121" priority="86">
       <formula>$Y21="Informe 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="130" priority="87">
+    <cfRule type="expression" dxfId="120" priority="87">
       <formula>$Y21="Informe 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="129" priority="88">
+    <cfRule type="expression" dxfId="119" priority="88">
       <formula>$Y21="Gráfico 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="128" priority="89">
+    <cfRule type="expression" dxfId="118" priority="89">
       <formula>$Y21="Gráfico 25"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="127" priority="90">
+    <cfRule type="expression" dxfId="117" priority="90">
       <formula>$Y21="Gráfico 24"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="91">
+    <cfRule type="expression" dxfId="116" priority="91">
       <formula>$Y21="Gráfico 23"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="92">
+    <cfRule type="expression" dxfId="115" priority="92">
       <formula>$Y21="Gráfico 22"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="93">
+    <cfRule type="expression" dxfId="114" priority="93">
       <formula>$Y21="Gráfico 21"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="94">
+    <cfRule type="expression" dxfId="113" priority="94">
       <formula>$Y21="Gráfico 20"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="95">
+    <cfRule type="expression" dxfId="112" priority="95">
       <formula>$Y21="Gráfico 18"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="96">
+    <cfRule type="expression" dxfId="111" priority="96">
       <formula>$Y21="Gráfico 19"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="97">
+    <cfRule type="expression" dxfId="110" priority="97">
       <formula>$Y21="Gráfico 17"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="119" priority="98">
+    <cfRule type="expression" dxfId="109" priority="98">
       <formula>$Y21="Gráfico 16"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="99">
+    <cfRule type="expression" dxfId="108" priority="99">
       <formula>$Y21="Gráfico 15"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="100">
+    <cfRule type="expression" dxfId="107" priority="100">
       <formula>$Y21="Gráfico 14"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="101">
+    <cfRule type="expression" dxfId="106" priority="101">
       <formula>$Y21="Gráfico 12"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="102">
+    <cfRule type="expression" dxfId="105" priority="102">
       <formula>$Y21="Gráfico 13"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="103">
+    <cfRule type="expression" dxfId="104" priority="103">
       <formula>$Y21="Gráfico 11"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="104">
+    <cfRule type="expression" dxfId="103" priority="104">
       <formula>$Y21="Gráfico 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="105">
+    <cfRule type="expression" dxfId="102" priority="105">
       <formula>$Y21="Gráfico 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="106">
+    <cfRule type="expression" dxfId="101" priority="106">
       <formula>$Y21="Gráfico 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="107">
+    <cfRule type="expression" dxfId="100" priority="107">
       <formula>$Y21="Gráfico 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="108">
+    <cfRule type="expression" dxfId="99" priority="108">
       <formula>$Y21="Gráfico 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="109">
+    <cfRule type="expression" dxfId="98" priority="109">
       <formula>$Y21="Gráfico 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="110">
+    <cfRule type="expression" dxfId="97" priority="110">
       <formula>$Y21="Gráfico 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="111">
+    <cfRule type="expression" dxfId="96" priority="111">
       <formula>$Y21="Gráfico 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="112">
+    <cfRule type="expression" dxfId="95" priority="112">
       <formula>$Y21="Gráfico 5"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O41:O44">
-    <cfRule type="expression" dxfId="104" priority="39">
+    <cfRule type="expression" dxfId="94" priority="39">
       <formula>$Z41="Reporte 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="40">
+    <cfRule type="expression" dxfId="93" priority="40">
       <formula>$Z41="Reporte 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="41">
+    <cfRule type="expression" dxfId="92" priority="41">
       <formula>$Z41="Informe 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="42">
+    <cfRule type="expression" dxfId="91" priority="42">
       <formula>$Z41="Informe 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="43">
+    <cfRule type="expression" dxfId="90" priority="43">
       <formula>$Z41="Informe 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="44">
+    <cfRule type="expression" dxfId="89" priority="44">
       <formula>$Z41="Informe 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="45">
+    <cfRule type="expression" dxfId="88" priority="45">
       <formula>$Z41="Informe 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="46">
+    <cfRule type="expression" dxfId="87" priority="46">
       <formula>$Z41="Informe 5"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="47">
+    <cfRule type="expression" dxfId="86" priority="47">
       <formula>$Z41="Informe 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="48">
+    <cfRule type="expression" dxfId="85" priority="48">
       <formula>$Z41="Informe 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="49">
+    <cfRule type="expression" dxfId="84" priority="49">
       <formula>$Z41="Informe 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="50">
+    <cfRule type="expression" dxfId="83" priority="50">
       <formula>$Z41="Informe 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="51">
+    <cfRule type="expression" dxfId="82" priority="51">
       <formula>$Z41="Gráfico 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="52">
+    <cfRule type="expression" dxfId="81" priority="52">
       <formula>$Z41="Gráfico 25"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="53">
+    <cfRule type="expression" dxfId="80" priority="53">
       <formula>$Z41="Gráfico 24"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="54">
+    <cfRule type="expression" dxfId="79" priority="54">
       <formula>$Z41="Gráfico 23"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="55">
+    <cfRule type="expression" dxfId="78" priority="55">
       <formula>$Z41="Gráfico 22"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="56">
+    <cfRule type="expression" dxfId="77" priority="56">
       <formula>$Z41="Gráfico 21"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="57">
+    <cfRule type="expression" dxfId="76" priority="57">
       <formula>$Z41="Gráfico 20"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="58">
+    <cfRule type="expression" dxfId="75" priority="58">
       <formula>$Z41="Gráfico 18"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="59">
+    <cfRule type="expression" dxfId="74" priority="59">
       <formula>$Z41="Gráfico 19"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="60">
+    <cfRule type="expression" dxfId="73" priority="60">
       <formula>$Z41="Gráfico 17"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="61">
+    <cfRule type="expression" dxfId="72" priority="61">
       <formula>$Z41="Gráfico 16"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="62">
+    <cfRule type="expression" dxfId="71" priority="62">
       <formula>$Z41="Gráfico 15"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="63">
+    <cfRule type="expression" dxfId="70" priority="63">
       <formula>$Z41="Gráfico 14"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="64">
+    <cfRule type="expression" dxfId="69" priority="64">
       <formula>$Z41="Gráfico 12"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="65">
+    <cfRule type="expression" dxfId="68" priority="65">
       <formula>$Z41="Gráfico 13"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="66">
+    <cfRule type="expression" dxfId="67" priority="66">
       <formula>$Z41="Gráfico 11"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="67">
+    <cfRule type="expression" dxfId="66" priority="67">
       <formula>$Z41="Gráfico 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="68">
+    <cfRule type="expression" dxfId="65" priority="68">
       <formula>$Z41="Gráfico 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="69">
+    <cfRule type="expression" dxfId="64" priority="69">
       <formula>$Z41="Gráfico 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="70">
+    <cfRule type="expression" dxfId="63" priority="70">
       <formula>$Z41="Gráfico 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="71">
+    <cfRule type="expression" dxfId="62" priority="71">
       <formula>$Z41="Gráfico 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="72">
+    <cfRule type="expression" dxfId="61" priority="72">
       <formula>$Z41="Gráfico 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="73">
+    <cfRule type="expression" dxfId="60" priority="73">
       <formula>$Z41="Gráfico 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="74">
+    <cfRule type="expression" dxfId="59" priority="74">
       <formula>$Z41="Gráfico 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="75">
+    <cfRule type="expression" dxfId="58" priority="75">
       <formula>$Z41="Gráfico 5"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O57:O59">
-    <cfRule type="expression" dxfId="67" priority="2">
+    <cfRule type="expression" dxfId="57" priority="2">
       <formula>$Z57="Reporte 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="3">
+    <cfRule type="expression" dxfId="56" priority="3">
       <formula>$Z57="Reporte 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="4">
+    <cfRule type="expression" dxfId="55" priority="4">
       <formula>$Z57="Informe 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="5">
+    <cfRule type="expression" dxfId="54" priority="5">
       <formula>$Z57="Informe 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="6">
+    <cfRule type="expression" dxfId="53" priority="6">
       <formula>$Z57="Informe 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="7">
+    <cfRule type="expression" dxfId="52" priority="7">
       <formula>$Z57="Informe 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="8">
+    <cfRule type="expression" dxfId="51" priority="8">
       <formula>$Z57="Informe 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="9">
+    <cfRule type="expression" dxfId="50" priority="9">
       <formula>$Z57="Informe 5"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="10">
+    <cfRule type="expression" dxfId="49" priority="10">
       <formula>$Z57="Informe 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="11">
+    <cfRule type="expression" dxfId="48" priority="11">
       <formula>$Z57="Informe 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="12">
+    <cfRule type="expression" dxfId="47" priority="12">
       <formula>$Z57="Informe 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="13">
+    <cfRule type="expression" dxfId="46" priority="13">
       <formula>$Z57="Informe 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="14">
+    <cfRule type="expression" dxfId="45" priority="14">
       <formula>$Z57="Gráfico 10"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="15">
+    <cfRule type="expression" dxfId="44" priority="15">
       <formula>$Z57="Gráfico 25"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="16">
+    <cfRule type="expression" dxfId="43" priority="16">
       <formula>$Z57="Gráfico 24"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="17">
+    <cfRule type="expression" dxfId="42" priority="17">
       <formula>$Z57="Gráfico 23"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="18">
+    <cfRule type="expression" dxfId="41" priority="18">
       <formula>$Z57="Gráfico 22"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="19">
+    <cfRule type="expression" dxfId="40" priority="19">
       <formula>$Z57="Gráfico 21"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="20">
+    <cfRule type="expression" dxfId="39" priority="20">
       <formula>$Z57="Gráfico 20"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="21">
+    <cfRule type="expression" dxfId="38" priority="21">
       <formula>$Z57="Gráfico 18"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="22">
+    <cfRule type="expression" dxfId="37" priority="22">
       <formula>$Z57="Gráfico 19"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="23">
+    <cfRule type="expression" dxfId="36" priority="23">
       <formula>$Z57="Gráfico 17"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="24">
+    <cfRule type="expression" dxfId="35" priority="24">
       <formula>$Z57="Gráfico 16"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="25">
+    <cfRule type="expression" dxfId="34" priority="25">
       <formula>$Z57="Gráfico 15"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="26">
+    <cfRule type="expression" dxfId="33" priority="26">
       <formula>$Z57="Gráfico 14"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="27">
+    <cfRule type="expression" dxfId="32" priority="27">
       <formula>$Z57="Gráfico 12"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="28">
+    <cfRule type="expression" dxfId="31" priority="28">
       <formula>$Z57="Gráfico 13"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="29">
+    <cfRule type="expression" dxfId="30" priority="29">
       <formula>$Z57="Gráfico 11"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="30">
+    <cfRule type="expression" dxfId="29" priority="30">
       <formula>$Z57="Gráfico 9"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="31">
+    <cfRule type="expression" dxfId="28" priority="31">
       <formula>$Z57="Gráfico 8"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="32">
+    <cfRule type="expression" dxfId="27" priority="32">
       <formula>$Z57="Gráfico 7"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="33">
+    <cfRule type="expression" dxfId="26" priority="33">
       <formula>$Z57="Gráfico 6"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="34">
+    <cfRule type="expression" dxfId="25" priority="34">
       <formula>$Z57="Gráfico 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="35">
+    <cfRule type="expression" dxfId="24" priority="35">
       <formula>$Z57="Gráfico 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="36">
+    <cfRule type="expression" dxfId="23" priority="36">
       <formula>$Z57="Gráfico 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="37">
+    <cfRule type="expression" dxfId="22" priority="37">
       <formula>$Z57="Gráfico 1"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="38">
+    <cfRule type="expression" dxfId="21" priority="38">
       <formula>$Z57="Gráfico 5"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:J96">
-    <cfRule type="cellIs" dxfId="30" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14343,17 +14239,18 @@
     <hyperlink ref="O41" r:id="rId55" xr:uid="{795FF98B-4C22-4CC4-9E8C-BF60C46E96ED}"/>
     <hyperlink ref="O57" r:id="rId56" xr:uid="{3FAD0F21-245E-4E3C-AFB4-6C25F5D7575F}"/>
     <hyperlink ref="O58" r:id="rId57" xr:uid="{23AB2DD9-566D-4A3F-9F29-B41183201E98}"/>
+    <hyperlink ref="O32" r:id="rId58" xr:uid="{7249FB21-DEBC-4F12-A9C4-114C9393C6E2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId58"/>
-  <drawing r:id="rId59"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId59"/>
+  <drawing r:id="rId60"/>
   <tableParts count="1">
-    <tablePart r:id="rId60"/>
+    <tablePart r:id="rId61"/>
   </tableParts>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{3A4CF648-6AED-40f4-86FF-DC5316D8AED3}">
       <x14:slicerList xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:slicer r:id="rId61"/>
+        <x14:slicer r:id="rId62"/>
       </x14:slicerList>
     </ext>
   </extLst>

</xml_diff>